<commit_message>
split & direct connexion change
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\VALEO_GA\VALEO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egos\Mon Drive\ORDI\PYTHON3\VALEO_GA\VALEO_gen_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DACBA-378D-4F1F-A347-E10C343701B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A5965D-32A9-4FD8-8B0B-50562EF14F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76680" yWindow="2610" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32460" yWindow="264" windowWidth="15000" windowHeight="10068" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="confs" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -838,8 +838,12 @@
       <c r="F9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>

</xml_diff>